<commit_message>
some  changes in html (capitals), adding wp and meal option to the form, changed the senders the mail id, cropped the regiatration id
</commit_message>
<xml_diff>
--- a/static/updated_field_names.xlsx
+++ b/static/updated_field_names.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -886,9 +886,230 @@
         <v>sdvascsASD</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>5fda7191-7378-4204-a3ad-da7b84184725</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Agniva</v>
+      </c>
+      <c r="C20" t="str">
+        <v>Bhattacharjee</v>
+      </c>
+      <c r="D20" t="str">
+        <v>bvbnm,</v>
+      </c>
+      <c r="E20" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F20" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G20" t="str">
+        <v>imagniva007@gmail.com</v>
+      </c>
+      <c r="H20" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I20" t="str">
+        <v>hgfcgvhbn</v>
+      </c>
+      <c r="J20" t="str">
+        <v>lkjkhghvhbn</v>
+      </c>
+      <c r="K20" t="str">
+        <v>knjhghcvb</v>
+      </c>
+      <c r="L20" t="str">
+        <v>mkjhgvhb</v>
+      </c>
+      <c r="M20" t="str">
+        <v>mjhgfcgvb</v>
+      </c>
+      <c r="N20" t="str">
+        <v>nbnvbvnm</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>3c693800-cee7-4dfc-b8d6-d86c77512b5f</v>
+      </c>
+      <c r="B21" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C21" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D21" t="str">
+        <v>biye to ei jonme hobe na</v>
+      </c>
+      <c r="E21" t="str">
+        <v>1947</v>
+      </c>
+      <c r="F21" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G21" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H21" t="str">
+        <v>0089-05-04</v>
+      </c>
+      <c r="I21" t="str">
+        <v>bekar jubok</v>
+      </c>
+      <c r="J21" t="str">
+        <v>Google</v>
+      </c>
+      <c r="K21" t="str">
+        <v>IAS OFFICER</v>
+      </c>
+      <c r="L21" t="str">
+        <v>All India Bakchod</v>
+      </c>
+      <c r="M21" t="str">
+        <v>nei kichu bhai</v>
+      </c>
+      <c r="N21" t="str">
+        <v>dfgtgrfedsx</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>BSS47afec85a74b</v>
+      </c>
+      <c r="B22" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C22" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D22" t="str">
+        <v>nei amar</v>
+      </c>
+      <c r="E22" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F22" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G22" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H22" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I22" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J22" t="str">
+        <v>google</v>
+      </c>
+      <c r="K22" t="str">
+        <v/>
+      </c>
+      <c r="L22" t="str">
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <v>sdsfdgfsvcs</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>BSS - c51ccd599251</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Suchi</v>
+      </c>
+      <c r="C23" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D23" t="str">
+        <v>nei amar</v>
+      </c>
+      <c r="E23" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F23" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G23" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H23" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I23" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J23" t="str">
+        <v>google</v>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <v/>
+      </c>
+      <c r="M23" t="str">
+        <v/>
+      </c>
+      <c r="N23" t="str">
+        <v>sdsfdgfsvcs1223</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>BSS - 9e614b382893</v>
+      </c>
+      <c r="B24" t="str">
+        <v>Suchi</v>
+      </c>
+      <c r="C24" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D24" t="str">
+        <v>nei amar</v>
+      </c>
+      <c r="E24" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F24" t="str">
+        <f>8420880979</f>
+        <v>08420880979</v>
+      </c>
+      <c r="G24" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H24" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I24" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J24" t="str">
+        <v>google</v>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <v/>
+      </c>
+      <c r="M24" t="str">
+        <v/>
+      </c>
+      <c r="N24" t="str">
+        <v>sdsfdgfsvcs1223</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N24"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change in email content
</commit_message>
<xml_diff>
--- a/static/updated_field_names.xlsx
+++ b/static/updated_field_names.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1123,7 +1123,6 @@
         <v>2020</v>
       </c>
       <c r="F25" t="str">
-        <f>8420880979</f>
         <v>08420880979</v>
       </c>
       <c r="G25" t="str">
@@ -1151,9 +1150,54 @@
         <v>something-something</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>BSS/d32409a3c007</v>
+      </c>
+      <c r="B26" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C26" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D26" t="str">
+        <v>kuch nhi hai</v>
+      </c>
+      <c r="E26" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F26" t="str">
+        <f>8420880979</f>
+        <v>08420880979</v>
+      </c>
+      <c r="G26" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H26" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I26" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J26" t="str">
+        <v>Google</v>
+      </c>
+      <c r="K26" t="str">
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <v>456465kjhgfg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N25"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N26"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
major changes in designing
</commit_message>
<xml_diff>
--- a/static/updated_field_names.xlsx
+++ b/static/updated_field_names.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1739,7 +1739,6 @@
         <v>02002</v>
       </c>
       <c r="F39" t="str">
-        <f>08420880979</f>
         <v>08420880979</v>
       </c>
       <c r="G39" t="str">
@@ -1767,9 +1766,274 @@
         <v>bnm,nmn mn.</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>BSS/3fca2c65e357</v>
+      </c>
+      <c r="B40" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C40" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D40" t="str">
+        <v>nei</v>
+      </c>
+      <c r="E40" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F40" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G40" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H40" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I40" t="str">
+        <v>cdvf</v>
+      </c>
+      <c r="J40" t="str">
+        <v/>
+      </c>
+      <c r="K40" t="str">
+        <v/>
+      </c>
+      <c r="L40" t="str">
+        <v/>
+      </c>
+      <c r="M40" t="str">
+        <v/>
+      </c>
+      <c r="N40" t="str">
+        <v>dvfgbdbfd</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>BSS/90242099a5fc</v>
+      </c>
+      <c r="B41" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C41" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D41" t="str">
+        <v>dfsdvsca</v>
+      </c>
+      <c r="E41" t="str">
+        <v>2021</v>
+      </c>
+      <c r="F41" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G41" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H41" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I41" t="str">
+        <v>sdvsfdvd</v>
+      </c>
+      <c r="J41" t="str">
+        <v/>
+      </c>
+      <c r="K41" t="str">
+        <v/>
+      </c>
+      <c r="L41" t="str">
+        <v/>
+      </c>
+      <c r="M41" t="str">
+        <v/>
+      </c>
+      <c r="N41" t="str">
+        <v>sdvsfbgdfsdv</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>BSS/29a5a21e81a8</v>
+      </c>
+      <c r="B42" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C42" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D42" t="str">
+        <v>dfsdvsca</v>
+      </c>
+      <c r="E42" t="str">
+        <v>2021</v>
+      </c>
+      <c r="F42" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G42" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H42" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I42" t="str">
+        <v>sdvsfdvd</v>
+      </c>
+      <c r="J42" t="str">
+        <v/>
+      </c>
+      <c r="K42" t="str">
+        <v/>
+      </c>
+      <c r="L42" t="str">
+        <v/>
+      </c>
+      <c r="M42" t="str">
+        <v/>
+      </c>
+      <c r="N42" t="str">
+        <v>sdvsfbgdfsdv</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>BSS/8e5c45e9e1d2</v>
+      </c>
+      <c r="B43" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C43" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D43" t="str">
+        <v>dfsdvsca</v>
+      </c>
+      <c r="E43" t="str">
+        <v>2021</v>
+      </c>
+      <c r="F43" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G43" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H43" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I43" t="str">
+        <v>sdvsfdvd</v>
+      </c>
+      <c r="J43" t="str">
+        <v/>
+      </c>
+      <c r="K43" t="str">
+        <v/>
+      </c>
+      <c r="L43" t="str">
+        <v/>
+      </c>
+      <c r="M43" t="str">
+        <v/>
+      </c>
+      <c r="N43" t="str">
+        <v>sdvsfbgdfsdv</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>BSS/16fe73826fad</v>
+      </c>
+      <c r="B44" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C44" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D44" t="str">
+        <v>dfsdvsca</v>
+      </c>
+      <c r="E44" t="str">
+        <v>2021</v>
+      </c>
+      <c r="F44" t="str">
+        <v>08420880979</v>
+      </c>
+      <c r="G44" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H44" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I44" t="str">
+        <v>sdvsfdvd</v>
+      </c>
+      <c r="J44" t="str">
+        <v/>
+      </c>
+      <c r="K44" t="str">
+        <v/>
+      </c>
+      <c r="L44" t="str">
+        <v/>
+      </c>
+      <c r="M44" t="str">
+        <v/>
+      </c>
+      <c r="N44" t="str">
+        <v>sdvsfbgdfsdv</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>BSS/9b6efdce74cd</v>
+      </c>
+      <c r="B45" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C45" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D45" t="str">
+        <v>biye hobe na er</v>
+      </c>
+      <c r="E45" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F45" t="str">
+        <f>08420880979</f>
+        <v>08420880979</v>
+      </c>
+      <c r="G45" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H45" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I45" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J45" t="str">
+        <v>Google</v>
+      </c>
+      <c r="K45" t="str">
+        <v/>
+      </c>
+      <c r="L45" t="str">
+        <v/>
+      </c>
+      <c r="M45" t="str">
+        <v/>
+      </c>
+      <c r="N45" t="str">
+        <v>dsfdvsdscabg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N39"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N45"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some changes in html and Encrypting the QR
</commit_message>
<xml_diff>
--- a/static/updated_field_names.xlsx
+++ b/static/updated_field_names.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2003,7 +2003,6 @@
         <v>2020</v>
       </c>
       <c r="F45" t="str">
-        <f>08420880979</f>
         <v>08420880979</v>
       </c>
       <c r="G45" t="str">
@@ -2031,9 +2030,54 @@
         <v>dsfdvsdscabg</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>BSS/9bf9433c0000</v>
+      </c>
+      <c r="B46" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C46" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D46" t="str">
+        <v>something</v>
+      </c>
+      <c r="E46" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F46" t="str">
+        <f>08420880979</f>
+        <v>08420880979</v>
+      </c>
+      <c r="G46" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H46" t="str">
+        <v>2002-01-21</v>
+      </c>
+      <c r="I46" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J46" t="str">
+        <v>Google</v>
+      </c>
+      <c r="K46" t="str">
+        <v/>
+      </c>
+      <c r="L46" t="str">
+        <v/>
+      </c>
+      <c r="M46" t="str">
+        <v/>
+      </c>
+      <c r="N46" t="str">
+        <v>aergty7u6543</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N45"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N46"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LOG IN BUTTON ACTIVATED
</commit_message>
<xml_diff>
--- a/static/updated_field_names.xlsx
+++ b/static/updated_field_names.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -2047,7 +2047,6 @@
         <v>2020</v>
       </c>
       <c r="F46" t="str">
-        <f>08420880979</f>
         <v>08420880979</v>
       </c>
       <c r="G46" t="str">
@@ -2075,9 +2074,54 @@
         <v>aergty7u6543</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>BSS/676f1e6bc5a4</v>
+      </c>
+      <c r="B47" t="str">
+        <v>AGNIVA</v>
+      </c>
+      <c r="C47" t="str">
+        <v>BHATTACHARJEE</v>
+      </c>
+      <c r="D47" t="str">
+        <v>nei</v>
+      </c>
+      <c r="E47" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F47" t="str">
+        <f>08420880979</f>
+        <v>08420880979</v>
+      </c>
+      <c r="G47" t="str">
+        <v>bhattacharjee.agniva.jobs@gmail.com</v>
+      </c>
+      <c r="H47" t="str">
+        <v>2202-01-21</v>
+      </c>
+      <c r="I47" t="str">
+        <v>IT</v>
+      </c>
+      <c r="J47" t="str">
+        <v>Google</v>
+      </c>
+      <c r="K47" t="str">
+        <v/>
+      </c>
+      <c r="L47" t="str">
+        <v/>
+      </c>
+      <c r="M47" t="str">
+        <v/>
+      </c>
+      <c r="N47" t="str">
+        <v>fvg67684yh</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N46"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>